<commit_message>
fix double counting of reading input tensor
</commit_message>
<xml_diff>
--- a/tests/traces/perf_model/normalization/normalization_layer_test_perf_report.xlsx
+++ b/tests/traces/perf_model/normalization/normalization_layer_test_perf_report.xlsx
@@ -4436,10 +4436,10 @@
         <v>0.001179648</v>
       </c>
       <c r="P2" t="n">
-        <v>2.3125</v>
+        <v>1.75</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4864864864864865</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
@@ -4447,10 +4447,10 @@
         </is>
       </c>
       <c r="S2" t="n">
-        <v>0.07438272891724061</v>
+        <v>0.05628963269412802</v>
       </c>
       <c r="T2" t="n">
-        <v>0.001332627723574454</v>
+        <v>0.001008475034056347</v>
       </c>
       <c r="U2" t="n">
         <v>0.03618619244622515</v>
@@ -4477,13 +4477,13 @@
         <v>25.478</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.0751044423338677</v>
+        <v>0.05683579419860258</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.07284490833614482</v>
+        <v>0.05512587657870418</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.0751988360817093</v>
+        <v>0.0569072273050773</v>
       </c>
       <c r="AF2" t="n">
         <v>0.03653729627053023</v>
@@ -4593,10 +4593,10 @@
         <v>0.001179648</v>
       </c>
       <c r="P3" t="n">
-        <v>2.0625</v>
+        <v>1.5625</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.72</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -4604,10 +4604,10 @@
         </is>
       </c>
       <c r="S3" t="n">
-        <v>0.08818391698080093</v>
+        <v>0.06680599771272798</v>
       </c>
       <c r="T3" t="n">
-        <v>0.002895810223053566</v>
+        <v>0.00219379562352543</v>
       </c>
       <c r="U3" t="n">
         <v>0.04810031835316414</v>
@@ -4634,13 +4634,13 @@
         <v>885.461</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.08792775939491394</v>
+        <v>0.06661193893554086</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.08542469524966731</v>
+        <v>0.06471567821944493</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.09119929629782153</v>
+        <v>0.06909037598319813</v>
       </c>
       <c r="AF3" t="n">
         <v>0.04796059603358942</v>
@@ -4907,10 +4907,10 @@
         <v>0.001179648</v>
       </c>
       <c r="P5" t="n">
-        <v>2.000076293945312</v>
+        <v>1.50006103515625</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.5624785431463949</v>
+        <v>0.749969483663588</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
@@ -4918,10 +4918,10 @@
         </is>
       </c>
       <c r="S5" t="n">
-        <v>0.1087745337676361</v>
+        <v>0.08158110778877121</v>
       </c>
       <c r="T5" t="n">
-        <v>0.01171947603161164</v>
+        <v>0.008789629375982646</v>
       </c>
       <c r="U5" t="n">
         <v>0.06118334128504826</v>
@@ -4948,13 +4948,13 @@
         <v>109.523</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1043140530904675</v>
+        <v>0.07823573877352762</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.09994022700514228</v>
+        <v>0.07495536086744072</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.1220693212072984</v>
+        <v>0.0915522237253453</v>
       </c>
       <c r="AF5" t="n">
         <v>0.05867441661202185</v>
@@ -5972,10 +5972,10 @@
         <v>0.001179648</v>
       </c>
       <c r="P12" t="n">
-        <v>2.000076293945312</v>
+        <v>1.50006103515625</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.5624785431463949</v>
+        <v>0.749969483663588</v>
       </c>
       <c r="R12" t="inlineStr">
         <is>
@@ -5983,10 +5983,10 @@
         </is>
       </c>
       <c r="S12" t="n">
-        <v>0.1547632122913547</v>
+        <v>0.1160727043946573</v>
       </c>
       <c r="T12" t="n">
-        <v>0.03294940711381235</v>
+        <v>0.02471211817896858</v>
       </c>
       <c r="U12" t="n">
         <v>0.08705098618229744</v>
@@ -6013,13 +6013,13 @@
         <v>449.741</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.1606256969334331</v>
+        <v>0.1204695790575916</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.1192760659816718</v>
+        <v>0.08945727697861705</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.1843878739589594</v>
+        <v>0.1382912571477634</v>
       </c>
       <c r="AF12" t="n">
         <v>0.09034850800299177</v>
@@ -6286,10 +6286,10 @@
         <v>0.001179648</v>
       </c>
       <c r="P14" t="n">
-        <v>2.00030517578125</v>
+        <v>1.500244140625</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.5624141824062491</v>
+        <v>0.7498779495524817</v>
       </c>
       <c r="R14" t="inlineStr">
         <is>
@@ -6297,10 +6297,10 @@
         </is>
       </c>
       <c r="S14" t="n">
-        <v>0.1848176224013407</v>
+        <v>0.13861462663244</v>
       </c>
       <c r="T14" t="n">
-        <v>0.00136160840308454</v>
+        <v>0.001021216688976221</v>
       </c>
       <c r="U14" t="n">
         <v>0.1039440519971169</v>
@@ -6327,13 +6327,13 @@
         <v>17.406</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.1843773137608378</v>
+        <v>0.138284391793287</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.1837306525235244</v>
+        <v>0.1377993909324209</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.1863449009196599</v>
+        <v>0.139760097171612</v>
       </c>
       <c r="AF14" t="n">
         <v>0.1036964161730621</v>
@@ -7190,10 +7190,10 @@
         <v>0.001179648</v>
       </c>
       <c r="P20" t="n">
-        <v>2.00244140625</v>
+        <v>1.501953125</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.5618141916605706</v>
+        <v>0.7490247074122237</v>
       </c>
       <c r="R20" t="inlineStr">
         <is>
@@ -7201,10 +7201,10 @@
         </is>
       </c>
       <c r="S20" t="n">
-        <v>0.3224022972886295</v>
+        <v>0.241821376849506</v>
       </c>
       <c r="T20" t="n">
-        <v>0.03970662502494311</v>
+        <v>0.0297823893140027</v>
       </c>
       <c r="U20" t="n">
         <v>0.1811301860407223</v>
@@ -7231,13 +7231,13 @@
         <v>620.236</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.3317551439592655</v>
+        <v>0.2488365820089493</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.2788541713248168</v>
+        <v>0.2091576276506063</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.3565975765818061</v>
+        <v>0.2674699208889626</v>
       </c>
       <c r="AF20" t="n">
         <v>0.186384748032711</v>
@@ -7661,10 +7661,10 @@
         <v>0.000524336</v>
       </c>
       <c r="P23" t="n">
-        <v>2.0001220703125</v>
+        <v>1.00006103515625</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.2500076289288984</v>
+        <v>0.5000152578577968</v>
       </c>
       <c r="R23" t="inlineStr">
         <is>
@@ -7672,10 +7672,10 @@
         </is>
       </c>
       <c r="S23" t="n">
-        <v>0.4134980203491416</v>
+        <v>0.2067490101745708</v>
       </c>
       <c r="T23" t="n">
-        <v>0.03704893546473456</v>
+        <v>0.01852446773236728</v>
       </c>
       <c r="U23" t="n">
         <v>0.1033776596342823</v>
@@ -7702,13 +7702,13 @@
         <v>1121.133</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.4188833079773747</v>
+        <v>0.2094416539886874</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.3740511573630584</v>
+        <v>0.1870255786815292</v>
       </c>
       <c r="AE23" t="n">
-        <v>0.4475595957069918</v>
+        <v>0.2237797978534959</v>
       </c>
       <c r="AF23" t="n">
         <v>0.104724022625317</v>
@@ -7975,10 +7975,10 @@
         <v>0.000524672</v>
       </c>
       <c r="P25" t="n">
-        <v>2.0009765625</v>
+        <v>1.00048828125</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.2500610053684724</v>
+        <v>0.5001220107369448</v>
       </c>
       <c r="R25" t="inlineStr">
         <is>
@@ -7986,10 +7986,10 @@
         </is>
       </c>
       <c r="S25" t="n">
-        <v>0.4742250986632798</v>
+        <v>0.2371125493316399</v>
       </c>
       <c r="T25" t="n">
-        <v>0.05884168768487954</v>
+        <v>0.02942084384243977</v>
       </c>
       <c r="U25" t="n">
         <v>0.1185852049427028</v>
@@ -8016,13 +8016,13 @@
         <v>1875.569</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.4895265946684894</v>
+        <v>0.2447632973342447</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.4092442331428571</v>
+        <v>0.2046221165714285</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.523904468178493</v>
+        <v>0.2619522340892465</v>
       </c>
       <c r="AF25" t="n">
         <v>0.1224115124174072</v>
@@ -10711,25 +10711,25 @@
         <v>0.001179648</v>
       </c>
       <c r="L3" t="n">
-        <v>2.3125</v>
+        <v>1.75</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4864864864864865</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="N3" t="n">
-        <v>0.07438272891724061</v>
+        <v>0.05628963269412802</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0751044423338677</v>
+        <v>0.05683579419860258</v>
       </c>
       <c r="P3" t="n">
-        <v>0.001332627723574454</v>
+        <v>0.001008475034056347</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.07284490833614482</v>
+        <v>0.05512587657870418</v>
       </c>
       <c r="R3" t="n">
-        <v>0.0751988360817093</v>
+        <v>0.0569072273050773</v>
       </c>
       <c r="S3" t="n">
         <v>0.03618619244622515</v>
@@ -11701,25 +11701,25 @@
         <v>0.001179648</v>
       </c>
       <c r="L9" t="n">
-        <v>2.0625</v>
+        <v>1.5625</v>
       </c>
       <c r="M9" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.72</v>
       </c>
       <c r="N9" t="n">
-        <v>0.08818391698080093</v>
+        <v>0.06680599771272798</v>
       </c>
       <c r="O9" t="n">
-        <v>0.08792775939491394</v>
+        <v>0.06661193893554086</v>
       </c>
       <c r="P9" t="n">
-        <v>0.002895810223053566</v>
+        <v>0.00219379562352543</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.08542469524966731</v>
+        <v>0.06471567821944493</v>
       </c>
       <c r="R9" t="n">
-        <v>0.09119929629782153</v>
+        <v>0.06909037598319813</v>
       </c>
       <c r="S9" t="n">
         <v>0.04810031835316414</v>
@@ -12196,25 +12196,25 @@
         <v>0.001179648</v>
       </c>
       <c r="L12" t="n">
-        <v>2.000076293945312</v>
+        <v>1.50006103515625</v>
       </c>
       <c r="M12" t="n">
-        <v>0.5624785431463949</v>
+        <v>0.749969483663588</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1087745337676361</v>
+        <v>0.08158110778877121</v>
       </c>
       <c r="O12" t="n">
-        <v>0.1043140530904675</v>
+        <v>0.07823573877352762</v>
       </c>
       <c r="P12" t="n">
-        <v>0.01171947603161164</v>
+        <v>0.008789629375982646</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.09994022700514228</v>
+        <v>0.07495536086744072</v>
       </c>
       <c r="R12" t="n">
-        <v>0.1220693212072984</v>
+        <v>0.0915522237253453</v>
       </c>
       <c r="S12" t="n">
         <v>0.06118334128504826</v>
@@ -12856,25 +12856,25 @@
         <v>0.001179648</v>
       </c>
       <c r="L16" t="n">
-        <v>2.000076293945312</v>
+        <v>1.50006103515625</v>
       </c>
       <c r="M16" t="n">
-        <v>0.5624785431463949</v>
+        <v>0.749969483663588</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1547632122913547</v>
+        <v>0.1160727043946573</v>
       </c>
       <c r="O16" t="n">
-        <v>0.1606256969334331</v>
+        <v>0.1204695790575916</v>
       </c>
       <c r="P16" t="n">
-        <v>0.03294940711381235</v>
+        <v>0.02471211817896858</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1192760659816718</v>
+        <v>0.08945727697861705</v>
       </c>
       <c r="R16" t="n">
-        <v>0.1843878739589594</v>
+        <v>0.1382912571477634</v>
       </c>
       <c r="S16" t="n">
         <v>0.08705098618229744</v>
@@ -13021,25 +13021,25 @@
         <v>0.001179648</v>
       </c>
       <c r="L17" t="n">
-        <v>2.00030517578125</v>
+        <v>1.500244140625</v>
       </c>
       <c r="M17" t="n">
-        <v>0.5624141824062491</v>
+        <v>0.7498779495524817</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1848176224013407</v>
+        <v>0.13861462663244</v>
       </c>
       <c r="O17" t="n">
-        <v>0.1843773137608378</v>
+        <v>0.138284391793287</v>
       </c>
       <c r="P17" t="n">
-        <v>0.00136160840308454</v>
+        <v>0.001021216688976221</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.1837306525235244</v>
+        <v>0.1377993909324209</v>
       </c>
       <c r="R17" t="n">
-        <v>0.1863449009196599</v>
+        <v>0.139760097171612</v>
       </c>
       <c r="S17" t="n">
         <v>0.1039440519971169</v>
@@ -13351,25 +13351,25 @@
         <v>0.001179648</v>
       </c>
       <c r="L19" t="n">
-        <v>2.00244140625</v>
+        <v>1.501953125</v>
       </c>
       <c r="M19" t="n">
-        <v>0.5618141916605706</v>
+        <v>0.7490247074122237</v>
       </c>
       <c r="N19" t="n">
-        <v>0.3224022972886295</v>
+        <v>0.241821376849506</v>
       </c>
       <c r="O19" t="n">
-        <v>0.3317551439592655</v>
+        <v>0.2488365820089493</v>
       </c>
       <c r="P19" t="n">
-        <v>0.03970662502494311</v>
+        <v>0.0297823893140027</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.2788541713248168</v>
+        <v>0.2091576276506063</v>
       </c>
       <c r="R19" t="n">
-        <v>0.3565975765818061</v>
+        <v>0.2674699208889626</v>
       </c>
       <c r="S19" t="n">
         <v>0.1811301860407223</v>
@@ -13681,25 +13681,25 @@
         <v>0.000524336</v>
       </c>
       <c r="L21" t="n">
-        <v>2.0001220703125</v>
+        <v>1.00006103515625</v>
       </c>
       <c r="M21" t="n">
-        <v>0.2500076289288984</v>
+        <v>0.5000152578577968</v>
       </c>
       <c r="N21" t="n">
-        <v>0.4134980203491416</v>
+        <v>0.2067490101745708</v>
       </c>
       <c r="O21" t="n">
-        <v>0.4188833079773747</v>
+        <v>0.2094416539886874</v>
       </c>
       <c r="P21" t="n">
-        <v>0.03704893546473456</v>
+        <v>0.01852446773236728</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.3740511573630584</v>
+        <v>0.1870255786815292</v>
       </c>
       <c r="R21" t="n">
-        <v>0.4475595957069918</v>
+        <v>0.2237797978534959</v>
       </c>
       <c r="S21" t="n">
         <v>0.1033776596342823</v>
@@ -13846,25 +13846,25 @@
         <v>0.000524672</v>
       </c>
       <c r="L22" t="n">
-        <v>2.0009765625</v>
+        <v>1.00048828125</v>
       </c>
       <c r="M22" t="n">
-        <v>0.2500610053684724</v>
+        <v>0.5001220107369448</v>
       </c>
       <c r="N22" t="n">
-        <v>0.4742250986632798</v>
+        <v>0.2371125493316399</v>
       </c>
       <c r="O22" t="n">
-        <v>0.4895265946684894</v>
+        <v>0.2447632973342447</v>
       </c>
       <c r="P22" t="n">
-        <v>0.05884168768487954</v>
+        <v>0.02942084384243977</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.4092442331428571</v>
+        <v>0.2046221165714285</v>
       </c>
       <c r="R22" t="n">
-        <v>0.523904468178493</v>
+        <v>0.2619522340892465</v>
       </c>
       <c r="S22" t="n">
         <v>0.1185852049427028</v>

</xml_diff>